<commit_message>
update testcase template doc
</commit_message>
<xml_diff>
--- a/testcases/template/资产管理.xlsx
+++ b/testcases/template/资产管理.xlsx
@@ -23,13 +23,13 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
   <si>
     <t>测试结果</t>
   </si>
@@ -1262,6 +1262,10 @@
   </si>
   <si>
     <t>添加资产管理用例</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表形式显示模型信息</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1289,6 +1293,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1297,6 +1302,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1304,6 +1310,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1311,6 +1318,7 @@
       <sz val="14"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1319,12 +1327,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -3594,7 +3604,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="J2:M6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -4183,7 +4193,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4464,8 +4474,8 @@
       <c r="C13" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>68</v>
+      <c r="D13" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="G13" s="16"/>
     </row>

</xml_diff>